<commit_message>
added another changes in the TC
</commit_message>
<xml_diff>
--- a/TestCase1.xlsx
+++ b/TestCase1.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7739DB87-61D6-4262-8B71-B9542E45C6A2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -18,8 +19,71 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>ID 1.1</t>
+  </si>
+  <si>
+    <t>KSTOLORZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CREATE ACCOUNT </t>
+  </si>
+  <si>
+    <t>NUMBER ID</t>
+  </si>
+  <si>
+    <t>AUTHOR</t>
+  </si>
+  <si>
+    <t>CATEGORY</t>
+  </si>
+  <si>
+    <t>TITLE</t>
+  </si>
+  <si>
+    <t>RESULT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRECONDITIONS
+</t>
+  </si>
+  <si>
+    <t>EXPECT RESULT</t>
+  </si>
+  <si>
+    <t>ENVIRONMENT</t>
+  </si>
+  <si>
+    <t>STEPS TO TEST</t>
+  </si>
+  <si>
+    <t>FINAL CONDITION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CREATING ACCOUNT TO THE GITHUB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">POSITIVE </t>
+  </si>
+  <si>
+    <t>1. Go to the  https://github.com/join</t>
+  </si>
+  <si>
+    <t>3. Click on the "Create an account" buton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Enter data for fields: Username, Email address and Password </t>
+  </si>
+  <si>
+    <t xml:space="preserve">user created account on the GITHUB </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -29,12 +93,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,11 +119,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +404,93 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="53.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>